<commit_message>
fonction schedule week begin
</commit_message>
<xml_diff>
--- a/documentation/journal de bord.xlsx
+++ b/documentation/journal de bord.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1555F0A5-A0E8-4039-A3FE-C1E49985705E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="2670" windowWidth="18870" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6345" yWindow="2670" windowWidth="18870" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">date </t>
   </si>
@@ -53,12 +52,15 @@
   </si>
   <si>
     <t>sprint review login et signin fonctionel</t>
+  </si>
+  <si>
+    <t>rencontre avec M Hurni pour une explication du fonctionement des Models (mon sauveur)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -376,11 +378,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +471,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44993</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>